<commit_message>
Suppression des references et correctifs 96ac5840dfc0f40661f77a6732bdab5ef2bee7f9
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-ActorPS.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-ActorPS.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-05T08:00:51+00:00</t>
+    <t>2025-05-05T11:54:16+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1379,10 +1379,10 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H7" t="s" s="2">
         <v>73</v>
@@ -1454,10 +1454,10 @@
         <v>104</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>73</v>

</xml_diff>

<commit_message>
creation datatype identifiant 350f501d4243fe231ea5debb5faf684c6ec3f7ec
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-ActorPS.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-ActorPS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="127">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-06T07:38:42+00:00</t>
+    <t>2025-05-06T13:57:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -253,43 +253,39 @@
     <t>ActorXDS</t>
   </si>
   <si>
-    <t>ActorPS.XCN1[x]</t>
+    <t>ActorPS.XCN1</t>
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/Identifiant
+</t>
+  </si>
+  <si>
+    <t>Identifiant de l'acteur</t>
+  </si>
+  <si>
+    <t>801234567890</t>
+  </si>
+  <si>
+    <t>ActorXDS.XCN1</t>
+  </si>
+  <si>
+    <t>author/assignedAuthor/id@extension</t>
+  </si>
+  <si>
+    <t>ActorPS.XCN1.value[x]</t>
   </si>
   <si>
     <t xml:space="preserve">https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/PSIdNat
 </t>
   </si>
   <si>
-    <t>Identifiant de l'acteur</t>
-  </si>
-  <si>
-    <t>801234567890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>ActorXDS.XCN1[x]</t>
-  </si>
-  <si>
-    <t>author/assignedAuthor/id@extension</t>
-  </si>
-  <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/PSIdNat
-https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/MatriculeINShttps://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/SNRstring {https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/IdentifiantSysteme}</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>IDNPS</t>
+    <t>Identifiant</t>
+  </si>
+  <si>
+    <t>Identifiant.value[x]</t>
   </si>
   <si>
     <t>ActorPS.XCN2</t>
@@ -299,6 +295,9 @@
 </t>
   </si>
   <si>
+    <t>Nom d'exercice du professionnel</t>
+  </si>
+  <si>
     <t>Nom d'exercice du professionnel, nom du patient, nom du système.</t>
   </si>
   <si>
@@ -309,6 +308,9 @@
   </si>
   <si>
     <t>ActorPS.XCN3</t>
+  </si>
+  <si>
+    <t>Prénom usuel de la personne</t>
   </si>
   <si>
     <t>Prénom usuel de la personne (par défaut le premier prénom), nom du modèle pour les dispositifs ou dénomination pour les autres systèmes.</t>
@@ -379,6 +381,9 @@
     <t>Type de nom : Valeur en fonction de l’auteur :  D, pour les personnes physiques, • U, pour les systèmes.</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
     <t>ActorXDS.XCN10</t>
   </si>
   <si>
@@ -388,16 +393,13 @@
     <t>Type d’identifiant</t>
   </si>
   <si>
+    <t>IDNPS</t>
+  </si>
+  <si>
     <t>ActorXDS.XCN13</t>
   </si>
   <si>
     <t>Valeur ne provenant pas de l’en-tête CDA</t>
-  </si>
-  <si>
-    <t>Nom d'exercice du professionnel</t>
-  </si>
-  <si>
-    <t>Prénom usuel de la personne</t>
   </si>
 </sst>
 </file>
@@ -702,7 +704,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AK12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -721,7 +723,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="197.09765625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="62.6484375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1038,40 +1040,42 @@
         <v>73</v>
       </c>
       <c r="AB3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AC3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AE3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF3" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="AC3" s="2"/>
-      <c r="AD3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE3" t="s" s="2">
+      <c r="AG3" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH3" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AK3" t="s" s="2">
         <v>85</v>
-      </c>
-      <c r="AF3" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AG3" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH3" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AI3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AJ3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK3" t="s" s="2">
-        <v>87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -1094,13 +1098,13 @@
         <v>73</v>
       </c>
       <c r="K4" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="L4" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="L4" t="s" s="2">
-        <v>82</v>
-      </c>
       <c r="M4" t="s" s="2">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1112,47 +1116,47 @@
         <v>73</v>
       </c>
       <c r="S4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="T4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="U4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="V4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="W4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="X4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Y4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Z4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AA4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AB4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AC4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AE4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF4" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="T4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="U4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="V4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="W4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="X4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Y4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Z4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AA4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AC4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AF4" t="s" s="2">
-        <v>86</v>
-      </c>
       <c r="AG4" t="s" s="2">
         <v>80</v>
       </c>
@@ -1166,15 +1170,15 @@
         <v>73</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -1197,13 +1201,13 @@
         <v>73</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1215,7 +1219,7 @@
         <v>73</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="T5" t="s" s="2">
         <v>73</v>
@@ -1254,7 +1258,7 @@
         <v>73</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>80</v>
@@ -1269,15 +1273,15 @@
         <v>73</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -1300,13 +1304,13 @@
         <v>73</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1357,7 +1361,7 @@
         <v>73</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>80</v>
@@ -1372,15 +1376,15 @@
         <v>73</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
@@ -1403,13 +1407,13 @@
         <v>73</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1460,7 +1464,7 @@
         <v>73</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>80</v>
@@ -1475,15 +1479,15 @@
         <v>73</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
@@ -1491,10 +1495,10 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s" s="2">
         <v>73</v>
@@ -1506,13 +1510,13 @@
         <v>73</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1563,13 +1567,13 @@
         <v>73</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AH8" t="s" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AI8" t="s" s="2">
         <v>73</v>
@@ -1578,15 +1582,15 @@
         <v>73</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
@@ -1594,10 +1598,10 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s" s="2">
         <v>73</v>
@@ -1609,13 +1613,13 @@
         <v>73</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1627,7 +1631,7 @@
         <v>73</v>
       </c>
       <c r="S9" t="s" s="2">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="T9" t="s" s="2">
         <v>73</v>
@@ -1666,13 +1670,13 @@
         <v>73</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="AG9" t="s" s="2">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="AH9" t="s" s="2">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="AI9" t="s" s="2">
         <v>73</v>
@@ -1681,15 +1685,15 @@
         <v>73</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
@@ -1712,13 +1716,13 @@
         <v>73</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1730,7 +1734,7 @@
         <v>73</v>
       </c>
       <c r="S10" t="s" s="2">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="T10" t="s" s="2">
         <v>73</v>
@@ -1769,7 +1773,7 @@
         <v>73</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>80</v>
@@ -1784,15 +1788,15 @@
         <v>73</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -1815,13 +1819,13 @@
         <v>73</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1833,7 +1837,7 @@
         <v>73</v>
       </c>
       <c r="S11" t="s" s="2">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="T11" t="s" s="2">
         <v>73</v>
@@ -1872,7 +1876,7 @@
         <v>73</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>80</v>
@@ -1887,15 +1891,15 @@
         <v>73</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -1918,13 +1922,13 @@
         <v>73</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1936,7 +1940,7 @@
         <v>73</v>
       </c>
       <c r="S12" t="s" s="2">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="T12" t="s" s="2">
         <v>73</v>
@@ -1975,7 +1979,7 @@
         <v>73</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>80</v>
@@ -1990,304 +1994,7 @@
         <v>73</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="G13" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="H13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="I13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="J13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="K13" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="L13" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Q13" s="2"/>
-      <c r="R13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="S13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="T13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="U13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="V13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="W13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="X13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Y13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Z13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AA13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AC13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AF13" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="AG13" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH13" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AI13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AJ13" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK13" t="s" s="2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="I14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="J14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="K14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L14" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Q14" s="2"/>
-      <c r="R14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="S14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="T14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="U14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="V14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="W14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="X14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Y14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Z14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AA14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AC14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AF14" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AG14" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AH14" s="2"/>
-      <c r="AI14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="I15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="J15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="K15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L15" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Q15" s="2"/>
-      <c r="R15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="S15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="T15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="U15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="V15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="W15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="X15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Y15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Z15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AA15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AC15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AF15" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AG15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AH15" s="2"/>
-      <c r="AI15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AJ15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK15" t="s" s="2">
-        <v>73</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>